<commit_message>
Logic to write API data to excel
</commit_message>
<xml_diff>
--- a/.data/Tenant_Utilization_Data_API.xlsx
+++ b/.data/Tenant_Utilization_Data_API.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/shreyas_risodkar_uipath_com/Documents/TAM India Initiatives/Hackweek 23/TAM_India_Hackweek_LicenseDataExtractor_Bot/.data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC104850F19D411C5ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F35B7FBB-582A-408C-ADE1-9885328FDA2B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="10" yWindow="120" windowWidth="19120" windowHeight="10220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>TenantName</t>
+  </si>
+  <si>
+    <t>FolderName</t>
+  </si>
+  <si>
+    <t>Trigger_Process_Name</t>
+  </si>
+  <si>
+    <t>Trigger_Schedule_CRON</t>
+  </si>
+  <si>
+    <t>Trigger_Runtime_type</t>
+  </si>
+  <si>
+    <t>Hackweek23</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>Hackweek 23 Testing</t>
+  </si>
+  <si>
+    <t>AZURE.VM.Conenct</t>
+  </si>
+  <si>
+    <t>0 0 0 1/1 * ? *</t>
+  </si>
+  <si>
+    <t>Unattended</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +374,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>